<commit_message>
Optimizacion de facturacion, plantilla, y creacion de Setup.py
</commit_message>
<xml_diff>
--- a/Plantilla.xlsx
+++ b/Plantilla.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rami\source\repos\Facturacion textil en Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rami\source\repos\Facturacion_textil_2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B04EAC-310B-4882-9EC3-5ACAB0D8DAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F666C63A-BF4C-4F65-AD8F-FC03B84245F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E6D90268-911F-4225-9558-77472726293D}"/>
   </bookViews>
@@ -246,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -322,6 +322,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -411,7 +417,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C2ECCD8-99A4-4784-96F1-732DE310D454}" name="Tabla1" displayName="Tabla1" ref="B4:G19" headerRowCount="0" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C2ECCD8-99A4-4784-96F1-732DE310D454}" name="Tabla1" displayName="Tabla1" ref="B4:G30" headerRowCount="0" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{486CD2FC-0311-46C9-9857-8F659D53A361}" name="Columna1" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{FC960386-1284-4A02-A4B0-0BCD92AA1140}" name="Columna2" dataDxfId="4"/>
@@ -713,7 +719,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -724,10 +730,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G44"/>
+  <dimension ref="B1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A11" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,90 +828,178 @@
       <c r="G9" s="11"/>
     </row>
     <row r="10" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="15"/>
       <c r="D10" s="8"/>
       <c r="E10" s="21"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="11"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="8"/>
       <c r="E11" s="21"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="11"/>
+      <c r="G11" s="26"/>
     </row>
     <row r="12" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="8"/>
       <c r="E12" s="21"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="11"/>
+      <c r="G12" s="26"/>
     </row>
     <row r="13" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="8"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="8"/>
       <c r="E13" s="21"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="12"/>
+      <c r="G13" s="26"/>
     </row>
     <row r="14" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="8"/>
       <c r="E14" s="21"/>
       <c r="F14" s="9"/>
-      <c r="G14" s="11"/>
+      <c r="G14" s="26"/>
     </row>
     <row r="15" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="8"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="8"/>
       <c r="E15" s="21"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="11"/>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-      <c r="C16" s="8"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="8"/>
       <c r="E16" s="21"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="11"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
-      <c r="C17" s="8"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="8"/>
       <c r="E17" s="21"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="22"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="26"/>
     </row>
     <row r="18" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="18"/>
-      <c r="C18" s="8"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="15"/>
       <c r="D18" s="8"/>
-      <c r="F18" s="19" t="s">
+      <c r="E18" s="21"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="26"/>
+    </row>
+    <row r="19" spans="2:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="2:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="27"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="26"/>
+    </row>
+    <row r="21" spans="2:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="2:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="2:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="2:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="2:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="2:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="2:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="2:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="22"/>
+    </row>
+    <row r="29" spans="2:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="18"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="F29" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G18" s="11"/>
-    </row>
-    <row r="19" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="20" t="s">
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="2:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="17"/>
-    </row>
-    <row r="44" spans="4:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D44" s="24"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="17"/>
+    </row>
+    <row r="55" spans="4:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D55" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.51181102362204722" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Creacion de iconos y facturacion
</commit_message>
<xml_diff>
--- a/Plantilla.xlsx
+++ b/Plantilla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rami\source\repos\Facturacion_textil_2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3404C181-416B-46F5-95BC-4DA9A2A62C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5F1497-6030-470E-9D1E-2C924DA3C1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E6D90268-911F-4225-9558-77472726293D}"/>
+    <workbookView xWindow="15615" yWindow="660" windowWidth="13095" windowHeight="13320" xr2:uid="{E6D90268-911F-4225-9558-77472726293D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -94,8 +94,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -263,7 +263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -322,25 +322,25 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -355,16 +355,10 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -373,34 +367,6 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="2" tint="-0.749992370372631"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="2" tint="-0.749992370372631"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -508,6 +474,34 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="2" tint="-0.749992370372631"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="2" tint="-0.749992370372631"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -526,15 +520,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2889775</xdr:colOff>
+      <xdr:colOff>2385511</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>256442</xdr:rowOff>
+      <xdr:rowOff>224118</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>55162</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>555360</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>296060</xdr:rowOff>
+      <xdr:rowOff>94355</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -563,8 +557,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3988813" y="7971692"/>
-          <a:ext cx="2213637" cy="1929964"/>
+          <a:off x="3483687" y="7922559"/>
+          <a:ext cx="2013467" cy="1752825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -577,13 +571,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C2ECCD8-99A4-4784-96F1-732DE310D454}" name="Tabla1" displayName="Tabla1" ref="A7:E26" headerRowCount="0" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C2ECCD8-99A4-4784-96F1-732DE310D454}" name="Tabla1" displayName="Tabla1" ref="A7:E26" headerRowCount="0" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{486CD2FC-0311-46C9-9857-8F659D53A361}" name="Columna1" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{F0BF9631-AD34-4D5D-A7A9-F2F923AF76AF}" name="Columna7" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{E0D71703-E7E5-4858-A12E-B478E3D3ECDD}" name="Columna3" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{2A4646E0-3DD8-493A-BA13-262098AD30C2}" name="Columna4" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{6668A6D6-3E80-4C77-A91A-1D32084D1BEE}" name="Columna6" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{486CD2FC-0311-46C9-9857-8F659D53A361}" name="Columna1" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{F0BF9631-AD34-4D5D-A7A9-F2F923AF76AF}" name="Columna7" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{E0D71703-E7E5-4858-A12E-B478E3D3ECDD}" name="Columna3" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{2A4646E0-3DD8-493A-BA13-262098AD30C2}" name="Columna4" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{6668A6D6-3E80-4C77-A91A-1D32084D1BEE}" name="Columna6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -878,7 +872,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -888,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0E44F0-6FC5-4593-B735-96347D41A42C}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A17" zoomScale="130" zoomScaleNormal="90" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,7 +915,7 @@
       <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="6"/>
@@ -932,7 +926,7 @@
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="32" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="6"/>
@@ -943,7 +937,7 @@
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="6"/>
@@ -1144,10 +1138,10 @@
       <c r="E31" s="26"/>
     </row>
     <row r="32" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D32" s="31" t="s">
+      <c r="D32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="32">
+      <c r="E32" s="31">
         <f>SUM(E8:E25)</f>
         <v>11100</v>
       </c>

</xml_diff>

<commit_message>
Adaptacion a facturacion textil
</commit_message>
<xml_diff>
--- a/Plantilla.xlsx
+++ b/Plantilla.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\source\repos\ramitules\Facturacion_textil_2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\source\repos\ramitules\Facturacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE16FC45-E0CB-462D-8AD2-647A119C1821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA471804-2467-4A5A-B715-C599CA217BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6D90268-911F-4225-9558-77472726293D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Cantidad</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Nombre:</t>
-  </si>
-  <si>
-    <t>Condición fiscal:</t>
   </si>
   <si>
     <t>Total:</t>
@@ -859,7 +856,7 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -903,9 +900,7 @@
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="A4" s="7"/>
       <c r="B4" s="3"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -1090,7 +1085,7 @@
     </row>
     <row r="31" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D31" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E31" s="29"/>
     </row>

</xml_diff>